<commit_message>
Switched out old Hex art for new
</commit_message>
<xml_diff>
--- a/Database/Currency.xlsx
+++ b/Database/Currency.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNI\Year 3\Group 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\GitHub\level-6-l6-group-1\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="8">
   <si>
     <t>Level</t>
   </si>
@@ -38,19 +38,22 @@
     <t>Stardust earned</t>
   </si>
   <si>
-    <t>Bouns for three star</t>
+    <t>Changes to -20 here</t>
   </si>
   <si>
-    <t>Bouns for Two star</t>
+    <t>Bonus for three star</t>
   </si>
   <si>
-    <t>Bouns for one star</t>
+    <t>Bonus for Two star</t>
+  </si>
+  <si>
+    <t>Bonus for one star</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -391,11 +394,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F201"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G201"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,6 +409,7 @@
     <col min="4" max="4" width="19.28515625" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -419,13 +423,13 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1601,7 +1605,7 @@
         <v>577.5</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -1626,7 +1630,7 @@
         <v>573.75</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -1651,7 +1655,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>0</v>
       </c>
@@ -1676,7 +1680,7 @@
         <v>566.25</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>0</v>
       </c>
@@ -1700,8 +1704,11 @@
         <f t="shared" si="2"/>
         <v>563.25</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -1726,7 +1733,7 @@
         <v>560.25</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>0</v>
       </c>
@@ -1751,7 +1758,7 @@
         <v>557.25</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>0</v>
       </c>
@@ -1776,7 +1783,7 @@
         <v>554.25</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>0</v>
       </c>
@@ -1801,7 +1808,7 @@
         <v>551.25</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -1826,7 +1833,7 @@
         <v>548.25</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>0</v>
       </c>
@@ -1851,7 +1858,7 @@
         <v>545.25</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>0</v>
       </c>
@@ -1876,7 +1883,7 @@
         <v>542.25</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>0</v>
       </c>
@@ -1901,7 +1908,7 @@
         <v>539.25</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>0</v>
       </c>
@@ -1926,7 +1933,7 @@
         <v>536.25</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -1951,7 +1958,7 @@
         <v>533.25</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>0</v>
       </c>
@@ -1976,7 +1983,7 @@
         <v>530.25</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>0</v>
       </c>

</xml_diff>